<commit_message>
Change Keys to stadistics month
</commit_message>
<xml_diff>
--- a/Data_storage/Storage/Historical_weather.xlsx
+++ b/Data_storage/Storage/Historical_weather.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -2892,6 +2892,1206 @@
         <v>0.45</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>18</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>00:00:05</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>45</v>
+      </c>
+      <c r="G82" t="n">
+        <v>1032</v>
+      </c>
+      <c r="H82" t="n">
+        <v>2.26</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>18</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>00:30:05</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>47</v>
+      </c>
+      <c r="G83" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H83" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>18</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>01:00:05</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>84</v>
+      </c>
+      <c r="G84" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H84" t="n">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>18</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>01:30:05</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>83</v>
+      </c>
+      <c r="G85" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H85" t="n">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>18</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>02:00:04</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>51</v>
+      </c>
+      <c r="G86" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H86" t="n">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>18</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>02:30:05</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>54</v>
+      </c>
+      <c r="G87" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H87" t="n">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>18</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>03:00:04</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>85</v>
+      </c>
+      <c r="G88" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H88" t="n">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>18</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>03:30:05</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>86</v>
+      </c>
+      <c r="G89" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H89" t="n">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>18</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>04:00:06</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>81</v>
+      </c>
+      <c r="G90" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H90" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>18</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>04:30:05</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>81</v>
+      </c>
+      <c r="G91" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H91" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>18</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>05:00:04</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>80</v>
+      </c>
+      <c r="G92" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H92" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>18</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>05:30:05</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>85</v>
+      </c>
+      <c r="G93" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H93" t="n">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>18</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>06:00:04</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>83</v>
+      </c>
+      <c r="G94" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H94" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>18</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>06:30:05</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>82</v>
+      </c>
+      <c r="G95" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H95" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>18</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>07:00:05</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>80</v>
+      </c>
+      <c r="G96" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H96" t="n">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>18</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>07:30:04</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>82</v>
+      </c>
+      <c r="G97" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H97" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>18</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>08:00:04</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>80</v>
+      </c>
+      <c r="G98" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>18</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>08:30:05</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>81</v>
+      </c>
+      <c r="G99" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H99" t="n">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>18</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>09:00:04</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>79</v>
+      </c>
+      <c r="G100" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H100" t="n">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>18</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>09:30:05</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>80</v>
+      </c>
+      <c r="G101" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H101" t="n">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>18</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>10:00:04</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>79</v>
+      </c>
+      <c r="G102" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H102" t="n">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>18</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>10:30:05</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>5.69</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>77</v>
+      </c>
+      <c r="G103" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H103" t="n">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>18</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>11:00:05</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>6.69</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>69</v>
+      </c>
+      <c r="G104" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>18</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>11:30:05</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>7.81</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>74</v>
+      </c>
+      <c r="G105" t="n">
+        <v>1030</v>
+      </c>
+      <c r="H105" t="n">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>18</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>12:00:05</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>9</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>63</v>
+      </c>
+      <c r="G106" t="n">
+        <v>1030</v>
+      </c>
+      <c r="H106" t="n">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>18</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>12:30:04</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>10</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>70</v>
+      </c>
+      <c r="G107" t="n">
+        <v>1028</v>
+      </c>
+      <c r="H107" t="n">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>18</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>13:00:05</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>10.88</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>69</v>
+      </c>
+      <c r="G108" t="n">
+        <v>1029</v>
+      </c>
+      <c r="H108" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>18</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>13:30:04</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>11.63</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0</v>
+      </c>
+      <c r="F109" t="n">
+        <v>67</v>
+      </c>
+      <c r="G109" t="n">
+        <v>1027</v>
+      </c>
+      <c r="H109" t="n">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>18</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>14:00:05</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>12.19</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>65</v>
+      </c>
+      <c r="G110" t="n">
+        <v>1027</v>
+      </c>
+      <c r="H110" t="n">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>18</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>14:30:04</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>12.69</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>65</v>
+      </c>
+      <c r="G111" t="n">
+        <v>1026</v>
+      </c>
+      <c r="H111" t="n">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>18</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>15:00:05</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>13.13</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>65</v>
+      </c>
+      <c r="G112" t="n">
+        <v>1026</v>
+      </c>
+      <c r="H112" t="n">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>18</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>15:30:04</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>13.31</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>66</v>
+      </c>
+      <c r="G113" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H113" t="n">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>18</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>16:00:05</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>13.19</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>68</v>
+      </c>
+      <c r="G114" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H114" t="n">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>18</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>16:30:05</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0</v>
+      </c>
+      <c r="F115" t="n">
+        <v>68</v>
+      </c>
+      <c r="G115" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H115" t="n">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>18</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>17:00:05</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>12.38</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>68</v>
+      </c>
+      <c r="G116" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H116" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>18</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>17:30:05</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>12.13</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>70</v>
+      </c>
+      <c r="G117" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>18</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>18:00:05</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>10.88</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" t="n">
+        <v>72</v>
+      </c>
+      <c r="G118" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H118" t="n">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>18</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>18:30:05</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>10.38</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" t="n">
+        <v>73</v>
+      </c>
+      <c r="G119" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H119" t="n">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>18</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>19:00:05</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>10.13</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" t="n">
+        <v>77</v>
+      </c>
+      <c r="G120" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H120" t="n">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>18</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>19:30:04</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>9.19</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>75</v>
+      </c>
+      <c r="G121" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H121" t="n">
+        <v>4.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>